<commit_message>
Include full test data for locations
</commit_message>
<xml_diff>
--- a/test_data/AddLocation/locations.xlsx
+++ b/test_data/AddLocation/locations.xlsx
@@ -5,22 +5,34 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pemar\Documents\FlowersResearch\Sparrow\Sparrow-CU-TRaIL\TRaIL-Data\AddLocation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pemar\Documents\FlowersResearch\Sparrow\Sparrow-CU-TRaIL\test_data\AddLocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761222D6-0EA0-45EB-BB51-163268531377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8DEA56D-153F-4D8E-8569-CC71EEA6E5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>21-00001</t>
   </si>
@@ -62,9 +74,6 @@
   </si>
   <si>
     <t>21-00014</t>
-  </si>
-  <si>
-    <t>23-00001</t>
   </si>
   <si>
     <t>Sample ID</t>
@@ -86,10 +95,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -419,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,97 +449,261 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>40.016019773996682</v>
+      </c>
+      <c r="C2">
+        <v>-105.25618106909128</v>
+      </c>
+      <c r="D2">
+        <v>1753.2133302031987</v>
+      </c>
+      <c r="E2">
+        <v>147.99480199174525</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>40.013542920924849</v>
+      </c>
+      <c r="C3">
+        <v>-105.25470464593657</v>
+      </c>
+      <c r="D3">
+        <v>1715.7635974635975</v>
+      </c>
+      <c r="E3">
+        <v>180.05712771131698</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>40.021837974701782</v>
+      </c>
+      <c r="C4">
+        <v>-105.25399594946768</v>
+      </c>
+      <c r="D4">
+        <v>1690.9275499614805</v>
+      </c>
+      <c r="E4">
+        <v>192.61463648358489</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>40.016148566089193</v>
+      </c>
+      <c r="C5">
+        <v>-105.25239552113064</v>
+      </c>
+      <c r="D5">
+        <v>1762.4123474751664</v>
+      </c>
+      <c r="E5">
+        <v>142.45407533726956</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>40.020431238355684</v>
+      </c>
+      <c r="C6">
+        <v>-105.25589224835406</v>
+      </c>
+      <c r="D6">
+        <v>1742.6391691332663</v>
+      </c>
+      <c r="E6">
+        <v>146.01521455537815</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>40.018073655376561</v>
+      </c>
+      <c r="C7">
+        <v>-105.25943306632337</v>
+      </c>
+      <c r="D7">
+        <v>1719.8830680775129</v>
+      </c>
+      <c r="E7">
+        <v>178.94100658385457</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>40.018019339388673</v>
+      </c>
+      <c r="C8">
+        <v>-105.2543351010837</v>
+      </c>
+      <c r="D8">
+        <v>1725.5239945842616</v>
+      </c>
+      <c r="E8">
+        <v>161.28128447627299</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>40.014255665674902</v>
+      </c>
+      <c r="C9">
+        <v>-105.25614613984045</v>
+      </c>
+      <c r="D9">
+        <v>1695.3701361203985</v>
+      </c>
+      <c r="E9">
+        <v>104.27472326119644</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>40.014356807963097</v>
+      </c>
+      <c r="C10">
+        <v>-105.25624078516704</v>
+      </c>
+      <c r="D10">
+        <v>1724.0625545729163</v>
+      </c>
+      <c r="E10">
+        <v>146.49614231927407</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11">
+        <v>40.014118147210318</v>
+      </c>
+      <c r="C11">
+        <v>-105.25169444864349</v>
+      </c>
+      <c r="D11">
+        <v>1758.5727686477501</v>
+      </c>
+      <c r="E11">
+        <v>153.959717426792</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12">
+        <v>40.01676321192857</v>
+      </c>
+      <c r="C12">
+        <v>-105.25636888315756</v>
+      </c>
+      <c r="D12">
+        <v>1755.592181515533</v>
+      </c>
+      <c r="E12">
+        <v>108.5249143416485</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13">
+        <v>40.015427695400398</v>
+      </c>
+      <c r="C13">
+        <v>-105.25473056288209</v>
+      </c>
+      <c r="D13">
+        <v>1748.5952835347541</v>
+      </c>
+      <c r="E13">
+        <v>151.11088434685578</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14">
+        <v>40.016160506104299</v>
+      </c>
+      <c r="C14">
+        <v>-105.259966614349</v>
+      </c>
+      <c r="D14">
+        <v>1695.6963712921606</v>
+      </c>
+      <c r="E14">
+        <v>189.30169152652914</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
+      <c r="B15">
+        <v>40.016098973807054</v>
+      </c>
+      <c r="C15">
+        <v>-105.25259209321005</v>
+      </c>
+      <c r="D15">
+        <v>1762.5258006718877</v>
+      </c>
+      <c r="E15">
+        <v>156.27872017820394</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>